<commit_message>
Completed Creating a Macro with the Macro Recorder
</commit_message>
<xml_diff>
--- a/30 - Macros/Excel103-AdvancedExercises.xlsx
+++ b/30 - Macros/Excel103-AdvancedExercises.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sint-my.sharepoint.com/personal/james_cox_unifii_co_uk/Documents/Documents/Training/Udemy/Excel/MicrosoftExcelFromBeginnerToAdvanced/30 - Macros/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="507" documentId="10_ncr:8000_{F5B4C794-7C2C-4A34-A8A1-2394A5AF9022}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DCFB8626-60E2-43A3-B6AE-3912AF226483}"/>
+  <xr:revisionPtr revIDLastSave="546" documentId="10_ncr:8000_{F5B4C794-7C2C-4A34-A8A1-2394A5AF9022}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A42AB33B-0DE7-41D5-8C2B-8680F410F822}"/>
   <bookViews>
     <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" firstSheet="16" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,6 +38,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'INDEX MATCH Master Emp List'!$A$1:$I$38</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="20" hidden="1">Macro!$A$1:$I$38</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Master Emp List'!$B$1:$I$38</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'SUMIF Function'!$A$2:$E$272</definedName>
     <definedName name="Monthly_Goal">'IF Function'!$I$2</definedName>
@@ -121,7 +122,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1538" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1547" uniqueCount="287">
   <si>
     <t>Monthly Goal:</t>
   </si>
@@ -973,13 +974,22 @@
   </si>
   <si>
     <t>EMP ID</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Ext</t>
+  </si>
+  <si>
+    <t>Pay</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="7">
+  <numFmts count="8">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="166" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
@@ -987,6 +997,7 @@
     <numFmt numFmtId="168" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="169" formatCode="0.00_);[Red]\(0.00\)"/>
     <numFmt numFmtId="170" formatCode="&quot;$&quot;#,##0.00;\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="172" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -1634,7 +1645,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="134">
+  <cellXfs count="138">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="169" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1969,17 +1980,23 @@
     <xf numFmtId="0" fontId="16" fillId="8" borderId="17" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="17" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="17" fillId="6" borderId="0" xfId="8" applyFont="1" applyFill="1"/>
+    <xf numFmtId="172" fontId="6" fillId="0" borderId="1" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
@@ -4904,10 +4921,10 @@
       <c r="C2" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="130" t="s">
+      <c r="E2" s="132" t="s">
         <v>166</v>
       </c>
-      <c r="F2" s="130"/>
+      <c r="F2" s="132"/>
     </row>
     <row r="3" spans="2:6" ht="13">
       <c r="B3" s="25" t="s">
@@ -4916,11 +4933,11 @@
       <c r="C3" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="131" t="str">
+      <c r="E3" s="130" t="str">
         <f>CONCATENATE(C3," ",B3)</f>
         <v>Howard Smith</v>
       </c>
-      <c r="F3" s="132"/>
+      <c r="F3" s="131"/>
     </row>
     <row r="4" spans="2:6" ht="13">
       <c r="B4" s="25" t="s">
@@ -4929,11 +4946,11 @@
       <c r="C4" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="131" t="str">
+      <c r="E4" s="130" t="str">
         <f>CONCATENATE(C4," ",B4)</f>
         <v>Joe Gonzales</v>
       </c>
-      <c r="F4" s="132"/>
+      <c r="F4" s="131"/>
     </row>
     <row r="5" spans="2:6" ht="13">
       <c r="B5" s="25" t="s">
@@ -4942,11 +4959,11 @@
       <c r="C5" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="131" t="str">
+      <c r="E5" s="130" t="str">
         <f t="shared" ref="E5:E18" si="0">CONCATENATE(C5," ",B5)</f>
         <v>Gail Scote</v>
       </c>
-      <c r="F5" s="132"/>
+      <c r="F5" s="131"/>
     </row>
     <row r="6" spans="2:6" ht="13">
       <c r="B6" s="25" t="s">
@@ -4955,11 +4972,11 @@
       <c r="C6" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="131" t="str">
+      <c r="E6" s="130" t="str">
         <f t="shared" si="0"/>
         <v>Sheryl Kane</v>
       </c>
-      <c r="F6" s="132"/>
+      <c r="F6" s="131"/>
     </row>
     <row r="7" spans="2:6" ht="13">
       <c r="B7" s="25" t="s">
@@ -4968,11 +4985,11 @@
       <c r="C7" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="131" t="str">
+      <c r="E7" s="130" t="str">
         <f t="shared" si="0"/>
         <v>Kendrick Hapsbuch</v>
       </c>
-      <c r="F7" s="132"/>
+      <c r="F7" s="131"/>
     </row>
     <row r="8" spans="2:6" ht="13">
       <c r="B8" s="25" t="s">
@@ -4981,11 +4998,11 @@
       <c r="C8" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="131" t="str">
+      <c r="E8" s="130" t="str">
         <f t="shared" si="0"/>
         <v>Mark Henders</v>
       </c>
-      <c r="F8" s="132"/>
+      <c r="F8" s="131"/>
     </row>
     <row r="9" spans="2:6" ht="13">
       <c r="B9" s="25" t="s">
@@ -4994,11 +5011,11 @@
       <c r="C9" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="131" t="str">
+      <c r="E9" s="130" t="str">
         <f t="shared" si="0"/>
         <v>Katie Atherton</v>
       </c>
-      <c r="F9" s="132"/>
+      <c r="F9" s="131"/>
     </row>
     <row r="10" spans="2:6" ht="13">
       <c r="B10" s="25" t="s">
@@ -5007,11 +5024,11 @@
       <c r="C10" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="131" t="str">
+      <c r="E10" s="130" t="str">
         <f t="shared" si="0"/>
         <v>Frank Bellwood</v>
       </c>
-      <c r="F10" s="132"/>
+      <c r="F10" s="131"/>
     </row>
     <row r="11" spans="2:6" ht="13">
       <c r="B11" s="25" t="s">
@@ -5020,11 +5037,11 @@
       <c r="C11" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="131" t="str">
+      <c r="E11" s="130" t="str">
         <f t="shared" si="0"/>
         <v>Linda Cooper</v>
       </c>
-      <c r="F11" s="132"/>
+      <c r="F11" s="131"/>
     </row>
     <row r="12" spans="2:6" ht="13">
       <c r="B12" s="25" t="s">
@@ -5033,11 +5050,11 @@
       <c r="C12" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="E12" s="131" t="str">
+      <c r="E12" s="130" t="str">
         <f t="shared" si="0"/>
         <v>Brent Cronwith</v>
       </c>
-      <c r="F12" s="132"/>
+      <c r="F12" s="131"/>
     </row>
     <row r="13" spans="2:6" ht="13">
       <c r="B13" s="25" t="s">
@@ -5046,11 +5063,11 @@
       <c r="C13" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="E13" s="131" t="str">
+      <c r="E13" s="130" t="str">
         <f t="shared" si="0"/>
         <v>Sandrae Simpson</v>
       </c>
-      <c r="F13" s="132"/>
+      <c r="F13" s="131"/>
     </row>
     <row r="14" spans="2:6" ht="13">
       <c r="B14" s="25" t="s">
@@ -5059,11 +5076,11 @@
       <c r="C14" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="E14" s="131" t="str">
+      <c r="E14" s="130" t="str">
         <f t="shared" si="0"/>
         <v>Randy Sindole</v>
       </c>
-      <c r="F14" s="132"/>
+      <c r="F14" s="131"/>
     </row>
     <row r="15" spans="2:6" ht="13">
       <c r="B15" s="25" t="s">
@@ -5072,11 +5089,11 @@
       <c r="C15" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="E15" s="131" t="str">
+      <c r="E15" s="130" t="str">
         <f t="shared" si="0"/>
         <v>Ellen Smith</v>
       </c>
-      <c r="F15" s="132"/>
+      <c r="F15" s="131"/>
     </row>
     <row r="16" spans="2:6" ht="13">
       <c r="B16" s="25" t="s">
@@ -5085,11 +5102,11 @@
       <c r="C16" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="E16" s="131" t="str">
+      <c r="E16" s="130" t="str">
         <f t="shared" si="0"/>
         <v>Tuome Vuanuo</v>
       </c>
-      <c r="F16" s="132"/>
+      <c r="F16" s="131"/>
     </row>
     <row r="17" spans="2:6" ht="13">
       <c r="B17" s="25" t="s">
@@ -5098,11 +5115,11 @@
       <c r="C17" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="E17" s="131" t="str">
+      <c r="E17" s="130" t="str">
         <f t="shared" si="0"/>
         <v>Tadeuz Szcznyck</v>
       </c>
-      <c r="F17" s="132"/>
+      <c r="F17" s="131"/>
     </row>
     <row r="18" spans="2:6" ht="13">
       <c r="B18" s="25" t="s">
@@ -5111,21 +5128,14 @@
       <c r="C18" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="E18" s="131" t="str">
+      <c r="E18" s="130" t="str">
         <f t="shared" si="0"/>
         <v>Tammy Wu</v>
       </c>
-      <c r="F18" s="132"/>
+      <c r="F18" s="131"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E4:F4"/>
@@ -5136,6 +5146,13 @@
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -11288,1051 +11305,1055 @@
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <sheetPr codeName="Sheet17"/>
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col min="2" max="2" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7265625" customWidth="1"/>
-    <col min="8" max="8" width="13.1796875" style="117" customWidth="1"/>
-    <col min="9" max="9" width="9.1796875" style="115"/>
+    <col min="1" max="1" width="11.6328125" customWidth="1"/>
+    <col min="2" max="2" width="15.54296875" customWidth="1"/>
+    <col min="3" max="3" width="15.36328125" customWidth="1"/>
+    <col min="4" max="4" width="9.6328125" customWidth="1"/>
+    <col min="5" max="5" width="11.26953125" customWidth="1"/>
+    <col min="6" max="6" width="8.7265625" customWidth="1"/>
+    <col min="7" max="7" width="13.36328125" customWidth="1"/>
+    <col min="8" max="8" width="14.6328125" style="117" customWidth="1"/>
+    <col min="9" max="9" width="9.6328125" style="115" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" s="7">
-        <v>1054</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="F1" s="7">
-        <v>148</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H1" s="116">
-        <v>33344</v>
-      </c>
-      <c r="I1" s="115">
-        <v>11.25</v>
+    <row r="1" spans="1:9" ht="15.5">
+      <c r="A1" s="134" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="134" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="134" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="134" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="134" t="s">
+        <v>284</v>
+      </c>
+      <c r="F1" s="134" t="s">
+        <v>285</v>
+      </c>
+      <c r="G1" s="134" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="135" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="136" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="7">
-        <v>1056</v>
+        <v>1054</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>27</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F2" s="7">
-        <v>121</v>
+        <v>148</v>
       </c>
       <c r="G2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H2" s="116">
-        <v>29153</v>
-      </c>
-      <c r="I2" s="115">
-        <v>12.25</v>
+      <c r="H2" s="137">
+        <v>33344</v>
+      </c>
+      <c r="I2" s="9">
+        <v>11.25</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="7">
-        <v>1067</v>
+        <v>1056</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>27</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F3" s="7">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G3" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H3" s="116">
-        <v>32040</v>
-      </c>
-      <c r="I3" s="115">
-        <v>14.55</v>
+      <c r="H3" s="137">
+        <v>29153</v>
+      </c>
+      <c r="I3" s="9">
+        <v>12.25</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="7">
-        <v>1075</v>
+        <v>1067</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="F4" s="7">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="H4" s="116">
-        <v>33823</v>
-      </c>
-      <c r="I4" s="115">
-        <v>11.25</v>
+        <v>29</v>
+      </c>
+      <c r="H4" s="137">
+        <v>32040</v>
+      </c>
+      <c r="I4" s="9">
+        <v>14.55</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="7">
-        <v>1078</v>
+        <v>1075</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="F5" s="7">
-        <v>101</v>
+        <v>126</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="H5" s="116">
-        <v>31503</v>
-      </c>
-      <c r="I5" s="115">
-        <v>10.199999999999999</v>
+      <c r="H5" s="137">
+        <v>33823</v>
+      </c>
+      <c r="I5" s="9">
+        <v>11.25</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="7">
-        <v>1152</v>
+        <v>1078</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F6" s="7">
-        <v>118</v>
+        <v>101</v>
       </c>
       <c r="G6" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="H6" s="116">
-        <v>32894</v>
-      </c>
-      <c r="I6" s="115">
-        <v>12.25</v>
+      <c r="H6" s="137">
+        <v>31503</v>
+      </c>
+      <c r="I6" s="9">
+        <v>10.199999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="7">
-        <v>1196</v>
+        <v>1152</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="F7" s="7">
-        <v>289</v>
+        <v>118</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H7" s="116">
-        <v>35886</v>
-      </c>
-      <c r="I7" s="115">
-        <v>9.9499999999999993</v>
+        <v>40</v>
+      </c>
+      <c r="H7" s="137">
+        <v>32894</v>
+      </c>
+      <c r="I7" s="9">
+        <v>12.25</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="7">
-        <v>1284</v>
+        <v>1196</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="F8" s="7">
-        <v>124</v>
+        <v>289</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H8" s="116">
-        <v>31051</v>
-      </c>
-      <c r="I8" s="115">
-        <v>12.3</v>
+        <v>24</v>
+      </c>
+      <c r="H8" s="137">
+        <v>35886</v>
+      </c>
+      <c r="I8" s="9">
+        <v>9.9499999999999993</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="7">
-        <v>1290</v>
+        <v>1284</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F9" s="7">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="H9" s="116">
-        <v>31050</v>
-      </c>
-      <c r="I9" s="115">
-        <v>13.25</v>
+        <v>29</v>
+      </c>
+      <c r="H9" s="137">
+        <v>31051</v>
+      </c>
+      <c r="I9" s="9">
+        <v>12.3</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="7">
-        <v>1293</v>
+        <v>1290</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F10" s="7">
-        <v>205</v>
+        <v>113</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H10" s="116">
-        <v>30939</v>
-      </c>
-      <c r="I10" s="115">
-        <v>10.199999999999999</v>
+        <v>40</v>
+      </c>
+      <c r="H10" s="137">
+        <v>31050</v>
+      </c>
+      <c r="I10" s="9">
+        <v>13.25</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="7">
-        <v>1299</v>
+        <v>1293</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F11" s="7">
-        <v>127</v>
+        <v>205</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H11" s="116">
-        <v>32863</v>
-      </c>
-      <c r="I11" s="115">
-        <v>12.2</v>
+        <v>24</v>
+      </c>
+      <c r="H11" s="137">
+        <v>30939</v>
+      </c>
+      <c r="I11" s="9">
+        <v>10.199999999999999</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="7">
-        <v>1302</v>
+        <v>1299</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F12" s="7">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="G12" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H12" s="116">
-        <v>30900</v>
-      </c>
-      <c r="I12" s="115">
-        <v>14.25</v>
+      <c r="H12" s="137">
+        <v>32863</v>
+      </c>
+      <c r="I12" s="9">
+        <v>12.2</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="7">
-        <v>1310</v>
+        <v>1302</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>25</v>
+        <v>66</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F13" s="7">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="G13" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H13" s="116">
-        <v>31689</v>
-      </c>
-      <c r="I13" s="115">
-        <v>11.5</v>
+      <c r="H13" s="137">
+        <v>30900</v>
+      </c>
+      <c r="I13" s="9">
+        <v>14.25</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="7">
-        <v>1329</v>
+        <v>1310</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>71</v>
+        <v>25</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>43</v>
+        <v>64</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F14" s="7">
-        <v>151</v>
+        <v>137</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="H14" s="116">
-        <v>32561</v>
-      </c>
-      <c r="I14" s="115">
-        <v>10.35</v>
+        <v>29</v>
+      </c>
+      <c r="H14" s="137">
+        <v>31689</v>
+      </c>
+      <c r="I14" s="9">
+        <v>11.5</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="7">
-        <v>1333</v>
+        <v>1329</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F15" s="7">
-        <v>122</v>
+        <v>151</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H15" s="116">
-        <v>32979</v>
-      </c>
-      <c r="I15" s="115">
-        <v>10.15</v>
+        <v>40</v>
+      </c>
+      <c r="H15" s="137">
+        <v>32561</v>
+      </c>
+      <c r="I15" s="9">
+        <v>10.35</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="7">
-        <v>1368</v>
+        <v>1333</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F16" s="7">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="H16" s="116">
-        <v>30386</v>
-      </c>
-      <c r="I16" s="115">
-        <v>12.25</v>
+        <v>24</v>
+      </c>
+      <c r="H16" s="137">
+        <v>32979</v>
+      </c>
+      <c r="I16" s="9">
+        <v>10.15</v>
       </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="7">
-        <v>1509</v>
+        <v>1368</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F17" s="7">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H17" s="116">
-        <v>31217</v>
-      </c>
-      <c r="I17" s="115">
-        <v>13.25</v>
+        <v>40</v>
+      </c>
+      <c r="H17" s="137">
+        <v>30386</v>
+      </c>
+      <c r="I17" s="9">
+        <v>12.25</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="7">
-        <v>1516</v>
+        <v>1509</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F18" s="7">
-        <v>105</v>
+        <v>135</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="H18" s="116">
-        <v>31112</v>
-      </c>
-      <c r="I18" s="115">
-        <v>9.5</v>
+        <v>29</v>
+      </c>
+      <c r="H18" s="137">
+        <v>31217</v>
+      </c>
+      <c r="I18" s="9">
+        <v>13.25</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="7">
-        <v>1529</v>
+        <v>1516</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F19" s="7">
-        <v>129</v>
+        <v>105</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H19" s="116">
-        <v>31805</v>
-      </c>
-      <c r="I19" s="115">
-        <v>11.3</v>
+        <v>40</v>
+      </c>
+      <c r="H19" s="137">
+        <v>31112</v>
+      </c>
+      <c r="I19" s="9">
+        <v>9.5</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="7">
-        <v>1656</v>
+        <v>1529</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F20" s="7">
-        <v>149</v>
+        <v>129</v>
       </c>
       <c r="G20" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H20" s="116">
-        <v>32125</v>
-      </c>
-      <c r="I20" s="115">
-        <v>12.35</v>
+      <c r="H20" s="137">
+        <v>31805</v>
+      </c>
+      <c r="I20" s="9">
+        <v>11.3</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="7">
-        <v>1672</v>
+        <v>1656</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D21" s="7" t="s">
         <v>64</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F21" s="7">
-        <v>114</v>
+        <v>149</v>
       </c>
       <c r="G21" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H21" s="116">
-        <v>32979</v>
-      </c>
-      <c r="I21" s="115">
-        <v>11.9</v>
+      <c r="H21" s="137">
+        <v>32125</v>
+      </c>
+      <c r="I21" s="9">
+        <v>12.35</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="7">
-        <v>1673</v>
+        <v>1672</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>53</v>
+        <v>93</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>38</v>
+        <v>64</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F22" s="7">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="H22" s="116">
-        <v>33688</v>
-      </c>
-      <c r="I22" s="115">
-        <v>11.85</v>
+        <v>29</v>
+      </c>
+      <c r="H22" s="137">
+        <v>32979</v>
+      </c>
+      <c r="I22" s="9">
+        <v>11.9</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="7">
-        <v>1676</v>
+        <v>1673</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>98</v>
+        <v>53</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F23" s="7">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H23" s="116">
-        <v>29885</v>
-      </c>
-      <c r="I23" s="115">
-        <v>10.75</v>
+        <v>40</v>
+      </c>
+      <c r="H23" s="137">
+        <v>33688</v>
+      </c>
+      <c r="I23" s="9">
+        <v>11.85</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="7">
-        <v>1721</v>
+        <v>1676</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F24" s="7">
-        <v>102</v>
+        <v>115</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H24" s="116">
-        <v>33091</v>
-      </c>
-      <c r="I24" s="115">
-        <v>9.75</v>
+        <v>29</v>
+      </c>
+      <c r="H24" s="137">
+        <v>29885</v>
+      </c>
+      <c r="I24" s="9">
+        <v>10.75</v>
       </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="7">
-        <v>1723</v>
+        <v>1721</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>46</v>
+        <v>101</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F25" s="7">
-        <v>145</v>
+        <v>102</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H25" s="116">
-        <v>28531</v>
-      </c>
-      <c r="I25" s="115">
-        <v>13.95</v>
+        <v>24</v>
+      </c>
+      <c r="H25" s="137">
+        <v>33091</v>
+      </c>
+      <c r="I25" s="9">
+        <v>9.75</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="7">
-        <v>1758</v>
+        <v>1723</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>106</v>
+        <v>46</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F26" s="7">
-        <v>107</v>
+        <v>145</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="H26" s="116">
-        <v>30028</v>
-      </c>
-      <c r="I26" s="115">
-        <v>11.2</v>
+        <v>29</v>
+      </c>
+      <c r="H26" s="137">
+        <v>28531</v>
+      </c>
+      <c r="I26" s="9">
+        <v>13.95</v>
       </c>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="7">
-        <v>1792</v>
+        <v>1758</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F27" s="7">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H27" s="116">
-        <v>33231</v>
-      </c>
-      <c r="I27" s="115">
-        <v>10.3</v>
+        <v>40</v>
+      </c>
+      <c r="H27" s="137">
+        <v>30028</v>
+      </c>
+      <c r="I27" s="9">
+        <v>11.2</v>
       </c>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="7">
-        <v>1814</v>
+        <v>1792</v>
       </c>
       <c r="B28" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="F28" s="7">
         <v>111</v>
       </c>
-      <c r="C28" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="F28" s="7">
-        <v>103</v>
-      </c>
       <c r="G28" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H28" s="116">
-        <v>32571</v>
-      </c>
-      <c r="I28" s="115">
-        <v>12.25</v>
+        <v>29</v>
+      </c>
+      <c r="H28" s="137">
+        <v>33231</v>
+      </c>
+      <c r="I28" s="9">
+        <v>10.3</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="7">
-        <v>1908</v>
+        <v>1814</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F29" s="7">
-        <v>152</v>
+        <v>103</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H29" s="116">
-        <v>30817</v>
-      </c>
-      <c r="I29" s="115">
-        <v>10.25</v>
+        <v>24</v>
+      </c>
+      <c r="H29" s="137">
+        <v>32571</v>
+      </c>
+      <c r="I29" s="9">
+        <v>12.25</v>
       </c>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="7">
-        <v>1931</v>
+        <v>1908</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F30" s="7">
-        <v>110</v>
+        <v>152</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="H30" s="116">
-        <v>32679</v>
-      </c>
-      <c r="I30" s="115">
-        <v>9.85</v>
+        <v>29</v>
+      </c>
+      <c r="H30" s="137">
+        <v>30817</v>
+      </c>
+      <c r="I30" s="9">
+        <v>10.25</v>
       </c>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="7">
-        <v>1960</v>
+        <v>1931</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>64</v>
+        <v>43</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F31" s="7">
-        <v>150</v>
+        <v>110</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H31" s="116">
-        <v>31729</v>
-      </c>
-      <c r="I31" s="115">
-        <v>11.65</v>
+        <v>40</v>
+      </c>
+      <c r="H31" s="137">
+        <v>32679</v>
+      </c>
+      <c r="I31" s="9">
+        <v>9.85</v>
       </c>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="7">
-        <v>1964</v>
+        <v>1960</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>43</v>
+        <v>64</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="F32" s="7">
-        <v>108</v>
+        <v>150</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="H32" s="116">
-        <v>33559</v>
-      </c>
-      <c r="I32" s="115">
-        <v>9.25</v>
+        <v>29</v>
+      </c>
+      <c r="H32" s="137">
+        <v>31729</v>
+      </c>
+      <c r="I32" s="9">
+        <v>11.65</v>
       </c>
     </row>
     <row r="33" spans="1:9">
       <c r="A33" s="7">
-        <v>1975</v>
+        <v>1964</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D33" s="7" t="s">
         <v>43</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F33" s="7">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="G33" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="H33" s="116">
-        <v>35125</v>
-      </c>
-      <c r="I33" s="115">
+      <c r="H33" s="137">
+        <v>33559</v>
+      </c>
+      <c r="I33" s="9">
         <v>9.25</v>
       </c>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="7">
-        <v>1983</v>
+        <v>1975</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F34" s="7">
-        <v>154</v>
+        <v>125</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H34" s="116">
-        <v>35609</v>
-      </c>
-      <c r="I34" s="115">
-        <v>11</v>
+        <v>40</v>
+      </c>
+      <c r="H34" s="137">
+        <v>35125</v>
+      </c>
+      <c r="I34" s="9">
+        <v>9.25</v>
       </c>
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="7">
-        <v>1990</v>
+        <v>1983</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>64</v>
+        <v>27</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F35" s="7">
-        <v>198</v>
+        <v>154</v>
       </c>
       <c r="G35" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H35" s="116">
-        <v>35840</v>
-      </c>
-      <c r="I35" s="115">
-        <v>10.95</v>
+      <c r="H35" s="137">
+        <v>35609</v>
+      </c>
+      <c r="I35" s="9">
+        <v>11</v>
       </c>
     </row>
     <row r="36" spans="1:9">
       <c r="A36" s="7">
-        <v>1995</v>
+        <v>1990</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>27</v>
+        <v>64</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="F36" s="7">
         <v>198</v>
@@ -12340,43 +12361,73 @@
       <c r="G36" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H36" s="116">
-        <v>35855</v>
-      </c>
-      <c r="I36" s="115">
-        <v>11.75</v>
+      <c r="H36" s="137">
+        <v>35840</v>
+      </c>
+      <c r="I36" s="9">
+        <v>10.95</v>
       </c>
     </row>
     <row r="37" spans="1:9">
       <c r="A37" s="7">
+        <v>1995</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="F37" s="7">
+        <v>198</v>
+      </c>
+      <c r="G37" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H37" s="137">
+        <v>35855</v>
+      </c>
+      <c r="I37" s="9">
+        <v>11.75</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38" s="7">
         <v>1999</v>
       </c>
-      <c r="B37" s="7" t="s">
+      <c r="B38" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="C37" s="7" t="s">
+      <c r="C38" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="D37" s="7" t="s">
+      <c r="D38" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="E37" s="7" t="s">
+      <c r="E38" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="F37" s="7">
+      <c r="F38" s="7">
         <v>428</v>
       </c>
-      <c r="G37" s="7" t="s">
+      <c r="G38" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="H37" s="116">
+      <c r="H38" s="137">
         <v>35981</v>
       </c>
-      <c r="I37" s="115">
+      <c r="I38" s="9">
         <v>10.15</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:I38" xr:uid="{00000000-0001-0000-1000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Completed Editing a Macro with VBA
</commit_message>
<xml_diff>
--- a/30 - Macros/Excel103-AdvancedExercises.xlsx
+++ b/30 - Macros/Excel103-AdvancedExercises.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sint-my.sharepoint.com/personal/james_cox_unifii_co_uk/Documents/Documents/Training/Udemy/Excel/MicrosoftExcelFromBeginnerToAdvanced/30 - Macros/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="546" documentId="10_ncr:8000_{F5B4C794-7C2C-4A34-A8A1-2394A5AF9022}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A42AB33B-0DE7-41D5-8C2B-8680F410F822}"/>
+  <xr:revisionPtr revIDLastSave="549" documentId="10_ncr:8000_{F5B4C794-7C2C-4A34-A8A1-2394A5AF9022}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1E55F84B-430F-4E36-9028-61E085010228}"/>
   <bookViews>
-    <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" firstSheet="16" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="16" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IF Function" sheetId="4" r:id="rId1"/>
@@ -34,7 +34,8 @@
     <sheet name="Data Table" sheetId="28" r:id="rId19"/>
     <sheet name="Scenarios" sheetId="29" r:id="rId20"/>
     <sheet name="Macro" sheetId="32" r:id="rId21"/>
-    <sheet name="Test Macro" sheetId="33" r:id="rId22"/>
+    <sheet name="Macro 2" sheetId="38" r:id="rId22"/>
+    <sheet name="Test Macro" sheetId="33" r:id="rId23"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'INDEX MATCH Master Emp List'!$A$1:$I$38</definedName>
@@ -122,7 +123,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1547" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1732" uniqueCount="287">
   <si>
     <t>Monthly Goal:</t>
   </si>
@@ -997,7 +998,7 @@
     <numFmt numFmtId="168" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="169" formatCode="0.00_);[Red]\(0.00\)"/>
     <numFmt numFmtId="170" formatCode="&quot;$&quot;#,##0.00;\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="172" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="171" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -1962,6 +1963,12 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="17" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="17" fillId="6" borderId="0" xfId="8" applyFont="1" applyFill="1"/>
+    <xf numFmtId="171" fontId="6" fillId="0" borderId="1" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -1980,23 +1987,17 @@
     <xf numFmtId="0" fontId="16" fillId="8" borderId="17" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="17" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="17" fillId="6" borderId="0" xfId="8" applyFont="1" applyFill="1"/>
-    <xf numFmtId="172" fontId="6" fillId="0" borderId="1" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
@@ -2710,14 +2711,14 @@
   <sheetData>
     <row r="1" spans="1:9" ht="13" thickBot="1"/>
     <row r="2" spans="1:9" ht="16" thickBot="1">
-      <c r="A2" s="127" t="s">
+      <c r="A2" s="131" t="s">
         <v>280</v>
       </c>
-      <c r="B2" s="127"/>
-      <c r="C2" s="127"/>
-      <c r="D2" s="127"/>
-      <c r="E2" s="127"/>
-      <c r="F2" s="127"/>
+      <c r="B2" s="131"/>
+      <c r="C2" s="131"/>
+      <c r="D2" s="131"/>
+      <c r="E2" s="131"/>
+      <c r="F2" s="131"/>
       <c r="H2" s="28" t="s">
         <v>0</v>
       </c>
@@ -2926,13 +2927,13 @@
       <c r="A11" s="49"/>
     </row>
     <row r="12" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A12" s="124" t="s">
+      <c r="A12" s="128" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="125"/>
-      <c r="C12" s="125"/>
-      <c r="D12" s="125"/>
-      <c r="E12" s="126"/>
+      <c r="B12" s="129"/>
+      <c r="C12" s="129"/>
+      <c r="D12" s="129"/>
+      <c r="E12" s="130"/>
       <c r="F12" s="3">
         <f>COUNTIF(H5:H9,"YES")</f>
         <v>3</v>
@@ -4921,10 +4922,10 @@
       <c r="C2" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="132" t="s">
+      <c r="E2" s="134" t="s">
         <v>166</v>
       </c>
-      <c r="F2" s="132"/>
+      <c r="F2" s="134"/>
     </row>
     <row r="3" spans="2:6" ht="13">
       <c r="B3" s="25" t="s">
@@ -4933,11 +4934,11 @@
       <c r="C3" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="130" t="str">
+      <c r="E3" s="135" t="str">
         <f>CONCATENATE(C3," ",B3)</f>
         <v>Howard Smith</v>
       </c>
-      <c r="F3" s="131"/>
+      <c r="F3" s="136"/>
     </row>
     <row r="4" spans="2:6" ht="13">
       <c r="B4" s="25" t="s">
@@ -4946,11 +4947,11 @@
       <c r="C4" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="130" t="str">
+      <c r="E4" s="135" t="str">
         <f>CONCATENATE(C4," ",B4)</f>
         <v>Joe Gonzales</v>
       </c>
-      <c r="F4" s="131"/>
+      <c r="F4" s="136"/>
     </row>
     <row r="5" spans="2:6" ht="13">
       <c r="B5" s="25" t="s">
@@ -4959,11 +4960,11 @@
       <c r="C5" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="130" t="str">
+      <c r="E5" s="135" t="str">
         <f t="shared" ref="E5:E18" si="0">CONCATENATE(C5," ",B5)</f>
         <v>Gail Scote</v>
       </c>
-      <c r="F5" s="131"/>
+      <c r="F5" s="136"/>
     </row>
     <row r="6" spans="2:6" ht="13">
       <c r="B6" s="25" t="s">
@@ -4972,11 +4973,11 @@
       <c r="C6" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="130" t="str">
+      <c r="E6" s="135" t="str">
         <f t="shared" si="0"/>
         <v>Sheryl Kane</v>
       </c>
-      <c r="F6" s="131"/>
+      <c r="F6" s="136"/>
     </row>
     <row r="7" spans="2:6" ht="13">
       <c r="B7" s="25" t="s">
@@ -4985,11 +4986,11 @@
       <c r="C7" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="130" t="str">
+      <c r="E7" s="135" t="str">
         <f t="shared" si="0"/>
         <v>Kendrick Hapsbuch</v>
       </c>
-      <c r="F7" s="131"/>
+      <c r="F7" s="136"/>
     </row>
     <row r="8" spans="2:6" ht="13">
       <c r="B8" s="25" t="s">
@@ -4998,11 +4999,11 @@
       <c r="C8" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="130" t="str">
+      <c r="E8" s="135" t="str">
         <f t="shared" si="0"/>
         <v>Mark Henders</v>
       </c>
-      <c r="F8" s="131"/>
+      <c r="F8" s="136"/>
     </row>
     <row r="9" spans="2:6" ht="13">
       <c r="B9" s="25" t="s">
@@ -5011,11 +5012,11 @@
       <c r="C9" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="130" t="str">
+      <c r="E9" s="135" t="str">
         <f t="shared" si="0"/>
         <v>Katie Atherton</v>
       </c>
-      <c r="F9" s="131"/>
+      <c r="F9" s="136"/>
     </row>
     <row r="10" spans="2:6" ht="13">
       <c r="B10" s="25" t="s">
@@ -5024,11 +5025,11 @@
       <c r="C10" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="130" t="str">
+      <c r="E10" s="135" t="str">
         <f t="shared" si="0"/>
         <v>Frank Bellwood</v>
       </c>
-      <c r="F10" s="131"/>
+      <c r="F10" s="136"/>
     </row>
     <row r="11" spans="2:6" ht="13">
       <c r="B11" s="25" t="s">
@@ -5037,11 +5038,11 @@
       <c r="C11" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="130" t="str">
+      <c r="E11" s="135" t="str">
         <f t="shared" si="0"/>
         <v>Linda Cooper</v>
       </c>
-      <c r="F11" s="131"/>
+      <c r="F11" s="136"/>
     </row>
     <row r="12" spans="2:6" ht="13">
       <c r="B12" s="25" t="s">
@@ -5050,11 +5051,11 @@
       <c r="C12" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="E12" s="130" t="str">
+      <c r="E12" s="135" t="str">
         <f t="shared" si="0"/>
         <v>Brent Cronwith</v>
       </c>
-      <c r="F12" s="131"/>
+      <c r="F12" s="136"/>
     </row>
     <row r="13" spans="2:6" ht="13">
       <c r="B13" s="25" t="s">
@@ -5063,11 +5064,11 @@
       <c r="C13" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="E13" s="130" t="str">
+      <c r="E13" s="135" t="str">
         <f t="shared" si="0"/>
         <v>Sandrae Simpson</v>
       </c>
-      <c r="F13" s="131"/>
+      <c r="F13" s="136"/>
     </row>
     <row r="14" spans="2:6" ht="13">
       <c r="B14" s="25" t="s">
@@ -5076,11 +5077,11 @@
       <c r="C14" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="E14" s="130" t="str">
+      <c r="E14" s="135" t="str">
         <f t="shared" si="0"/>
         <v>Randy Sindole</v>
       </c>
-      <c r="F14" s="131"/>
+      <c r="F14" s="136"/>
     </row>
     <row r="15" spans="2:6" ht="13">
       <c r="B15" s="25" t="s">
@@ -5089,11 +5090,11 @@
       <c r="C15" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="E15" s="130" t="str">
+      <c r="E15" s="135" t="str">
         <f t="shared" si="0"/>
         <v>Ellen Smith</v>
       </c>
-      <c r="F15" s="131"/>
+      <c r="F15" s="136"/>
     </row>
     <row r="16" spans="2:6" ht="13">
       <c r="B16" s="25" t="s">
@@ -5102,11 +5103,11 @@
       <c r="C16" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="E16" s="130" t="str">
+      <c r="E16" s="135" t="str">
         <f t="shared" si="0"/>
         <v>Tuome Vuanuo</v>
       </c>
-      <c r="F16" s="131"/>
+      <c r="F16" s="136"/>
     </row>
     <row r="17" spans="2:6" ht="13">
       <c r="B17" s="25" t="s">
@@ -5115,11 +5116,11 @@
       <c r="C17" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="E17" s="130" t="str">
+      <c r="E17" s="135" t="str">
         <f t="shared" si="0"/>
         <v>Tadeuz Szcznyck</v>
       </c>
-      <c r="F17" s="131"/>
+      <c r="F17" s="136"/>
     </row>
     <row r="18" spans="2:6" ht="13">
       <c r="B18" s="25" t="s">
@@ -5128,14 +5129,21 @@
       <c r="C18" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="E18" s="130" t="str">
+      <c r="E18" s="135" t="str">
         <f t="shared" si="0"/>
         <v>Tammy Wu</v>
       </c>
-      <c r="F18" s="131"/>
+      <c r="F18" s="136"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E4:F4"/>
@@ -5146,13 +5154,6 @@
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5184,14 +5185,14 @@
   <sheetData>
     <row r="1" spans="1:9" ht="13" thickBot="1"/>
     <row r="2" spans="1:9" ht="16" thickBot="1">
-      <c r="A2" s="127" t="s">
+      <c r="A2" s="131" t="s">
         <v>222</v>
       </c>
-      <c r="B2" s="127"/>
-      <c r="C2" s="127"/>
-      <c r="D2" s="127"/>
-      <c r="E2" s="127"/>
-      <c r="F2" s="127"/>
+      <c r="B2" s="131"/>
+      <c r="C2" s="131"/>
+      <c r="D2" s="131"/>
+      <c r="E2" s="131"/>
+      <c r="F2" s="131"/>
       <c r="H2" s="28" t="s">
         <v>0</v>
       </c>
@@ -5410,13 +5411,13 @@
     </row>
     <row r="13" spans="1:9" ht="3" customHeight="1"/>
     <row r="14" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A14" s="124" t="s">
+      <c r="A14" s="128" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="125"/>
-      <c r="C14" s="125"/>
-      <c r="D14" s="125"/>
-      <c r="E14" s="126"/>
+      <c r="B14" s="129"/>
+      <c r="C14" s="129"/>
+      <c r="D14" s="129"/>
+      <c r="E14" s="130"/>
       <c r="F14" s="3">
         <f>COUNTIF(H5:H9, "YES")</f>
         <v>3</v>
@@ -5486,14 +5487,14 @@
   <sheetData>
     <row r="1" spans="1:9" ht="13" thickBot="1"/>
     <row r="2" spans="1:9" ht="16" thickBot="1">
-      <c r="A2" s="127" t="s">
+      <c r="A2" s="131" t="s">
         <v>222</v>
       </c>
-      <c r="B2" s="127"/>
-      <c r="C2" s="127"/>
-      <c r="D2" s="127"/>
-      <c r="E2" s="127"/>
-      <c r="F2" s="127"/>
+      <c r="B2" s="131"/>
+      <c r="C2" s="131"/>
+      <c r="D2" s="131"/>
+      <c r="E2" s="131"/>
+      <c r="F2" s="131"/>
       <c r="H2" s="28" t="s">
         <v>0</v>
       </c>
@@ -5713,13 +5714,13 @@
     </row>
     <row r="13" spans="1:9" ht="3" customHeight="1"/>
     <row r="14" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A14" s="124" t="s">
+      <c r="A14" s="128" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="125"/>
-      <c r="C14" s="125"/>
-      <c r="D14" s="125"/>
-      <c r="E14" s="126"/>
+      <c r="B14" s="129"/>
+      <c r="C14" s="129"/>
+      <c r="D14" s="129"/>
+      <c r="E14" s="130"/>
       <c r="F14" s="3">
         <f>COUNTIF(H5:H9, "YES")</f>
         <v>3</v>
@@ -11231,10 +11232,10 @@
       </c>
     </row>
     <row r="10" spans="2:7" ht="13">
-      <c r="B10" s="133" t="s">
+      <c r="B10" s="137" t="s">
         <v>259</v>
       </c>
-      <c r="C10" s="133"/>
+      <c r="C10" s="137"/>
     </row>
     <row r="11" spans="2:7" ht="13">
       <c r="B11" s="113" t="s">
@@ -11307,8 +11308,8 @@
   <sheetPr codeName="Sheet17"/>
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
@@ -11325,31 +11326,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.5">
-      <c r="A1" s="134" t="s">
+      <c r="A1" s="124" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="134" t="s">
+      <c r="B1" s="124" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="134" t="s">
+      <c r="C1" s="124" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="134" t="s">
+      <c r="D1" s="124" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="134" t="s">
+      <c r="E1" s="124" t="s">
         <v>284</v>
       </c>
-      <c r="F1" s="134" t="s">
+      <c r="F1" s="124" t="s">
         <v>285</v>
       </c>
-      <c r="G1" s="134" t="s">
+      <c r="G1" s="124" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="135" t="s">
+      <c r="H1" s="125" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="136" t="s">
+      <c r="I1" s="126" t="s">
         <v>286</v>
       </c>
     </row>
@@ -11375,7 +11376,7 @@
       <c r="G2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H2" s="137">
+      <c r="H2" s="127">
         <v>33344</v>
       </c>
       <c r="I2" s="9">
@@ -11404,7 +11405,7 @@
       <c r="G3" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H3" s="137">
+      <c r="H3" s="127">
         <v>29153</v>
       </c>
       <c r="I3" s="9">
@@ -11433,7 +11434,7 @@
       <c r="G4" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="137">
+      <c r="H4" s="127">
         <v>32040</v>
       </c>
       <c r="I4" s="9">
@@ -11462,7 +11463,7 @@
       <c r="G5" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="H5" s="137">
+      <c r="H5" s="127">
         <v>33823</v>
       </c>
       <c r="I5" s="9">
@@ -11491,7 +11492,7 @@
       <c r="G6" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="H6" s="137">
+      <c r="H6" s="127">
         <v>31503</v>
       </c>
       <c r="I6" s="9">
@@ -11520,7 +11521,7 @@
       <c r="G7" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="H7" s="137">
+      <c r="H7" s="127">
         <v>32894</v>
       </c>
       <c r="I7" s="9">
@@ -11549,7 +11550,7 @@
       <c r="G8" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="H8" s="137">
+      <c r="H8" s="127">
         <v>35886</v>
       </c>
       <c r="I8" s="9">
@@ -11578,7 +11579,7 @@
       <c r="G9" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H9" s="137">
+      <c r="H9" s="127">
         <v>31051</v>
       </c>
       <c r="I9" s="9">
@@ -11607,7 +11608,7 @@
       <c r="G10" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="H10" s="137">
+      <c r="H10" s="127">
         <v>31050</v>
       </c>
       <c r="I10" s="9">
@@ -11636,7 +11637,7 @@
       <c r="G11" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="H11" s="137">
+      <c r="H11" s="127">
         <v>30939</v>
       </c>
       <c r="I11" s="9">
@@ -11665,7 +11666,7 @@
       <c r="G12" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H12" s="137">
+      <c r="H12" s="127">
         <v>32863</v>
       </c>
       <c r="I12" s="9">
@@ -11694,7 +11695,7 @@
       <c r="G13" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H13" s="137">
+      <c r="H13" s="127">
         <v>30900</v>
       </c>
       <c r="I13" s="9">
@@ -11723,7 +11724,7 @@
       <c r="G14" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H14" s="137">
+      <c r="H14" s="127">
         <v>31689</v>
       </c>
       <c r="I14" s="9">
@@ -11752,7 +11753,7 @@
       <c r="G15" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="H15" s="137">
+      <c r="H15" s="127">
         <v>32561</v>
       </c>
       <c r="I15" s="9">
@@ -11781,7 +11782,7 @@
       <c r="G16" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="H16" s="137">
+      <c r="H16" s="127">
         <v>32979</v>
       </c>
       <c r="I16" s="9">
@@ -11810,7 +11811,7 @@
       <c r="G17" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="H17" s="137">
+      <c r="H17" s="127">
         <v>30386</v>
       </c>
       <c r="I17" s="9">
@@ -11839,7 +11840,7 @@
       <c r="G18" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H18" s="137">
+      <c r="H18" s="127">
         <v>31217</v>
       </c>
       <c r="I18" s="9">
@@ -11868,7 +11869,7 @@
       <c r="G19" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="H19" s="137">
+      <c r="H19" s="127">
         <v>31112</v>
       </c>
       <c r="I19" s="9">
@@ -11897,7 +11898,7 @@
       <c r="G20" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H20" s="137">
+      <c r="H20" s="127">
         <v>31805</v>
       </c>
       <c r="I20" s="9">
@@ -11926,7 +11927,7 @@
       <c r="G21" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H21" s="137">
+      <c r="H21" s="127">
         <v>32125</v>
       </c>
       <c r="I21" s="9">
@@ -11955,7 +11956,7 @@
       <c r="G22" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H22" s="137">
+      <c r="H22" s="127">
         <v>32979</v>
       </c>
       <c r="I22" s="9">
@@ -11984,7 +11985,7 @@
       <c r="G23" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="H23" s="137">
+      <c r="H23" s="127">
         <v>33688</v>
       </c>
       <c r="I23" s="9">
@@ -12013,7 +12014,7 @@
       <c r="G24" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H24" s="137">
+      <c r="H24" s="127">
         <v>29885</v>
       </c>
       <c r="I24" s="9">
@@ -12042,7 +12043,7 @@
       <c r="G25" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="H25" s="137">
+      <c r="H25" s="127">
         <v>33091</v>
       </c>
       <c r="I25" s="9">
@@ -12071,7 +12072,7 @@
       <c r="G26" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H26" s="137">
+      <c r="H26" s="127">
         <v>28531</v>
       </c>
       <c r="I26" s="9">
@@ -12100,7 +12101,7 @@
       <c r="G27" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="H27" s="137">
+      <c r="H27" s="127">
         <v>30028</v>
       </c>
       <c r="I27" s="9">
@@ -12129,7 +12130,7 @@
       <c r="G28" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H28" s="137">
+      <c r="H28" s="127">
         <v>33231</v>
       </c>
       <c r="I28" s="9">
@@ -12158,7 +12159,7 @@
       <c r="G29" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="H29" s="137">
+      <c r="H29" s="127">
         <v>32571</v>
       </c>
       <c r="I29" s="9">
@@ -12187,7 +12188,7 @@
       <c r="G30" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H30" s="137">
+      <c r="H30" s="127">
         <v>30817</v>
       </c>
       <c r="I30" s="9">
@@ -12216,7 +12217,7 @@
       <c r="G31" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="H31" s="137">
+      <c r="H31" s="127">
         <v>32679</v>
       </c>
       <c r="I31" s="9">
@@ -12245,7 +12246,7 @@
       <c r="G32" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H32" s="137">
+      <c r="H32" s="127">
         <v>31729</v>
       </c>
       <c r="I32" s="9">
@@ -12274,7 +12275,7 @@
       <c r="G33" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="H33" s="137">
+      <c r="H33" s="127">
         <v>33559</v>
       </c>
       <c r="I33" s="9">
@@ -12303,7 +12304,7 @@
       <c r="G34" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="H34" s="137">
+      <c r="H34" s="127">
         <v>35125</v>
       </c>
       <c r="I34" s="9">
@@ -12332,7 +12333,7 @@
       <c r="G35" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H35" s="137">
+      <c r="H35" s="127">
         <v>35609</v>
       </c>
       <c r="I35" s="9">
@@ -12361,7 +12362,7 @@
       <c r="G36" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H36" s="137">
+      <c r="H36" s="127">
         <v>35840</v>
       </c>
       <c r="I36" s="9">
@@ -12390,7 +12391,7 @@
       <c r="G37" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H37" s="137">
+      <c r="H37" s="127">
         <v>35855</v>
       </c>
       <c r="I37" s="9">
@@ -12419,7 +12420,7 @@
       <c r="G38" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="H38" s="137">
+      <c r="H38" s="127">
         <v>35981</v>
       </c>
       <c r="I38" s="9">
@@ -12433,6 +12434,1100 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9E1E704-C79A-4573-B58C-DA8EC512683B}">
+  <sheetPr codeName="Sheet23"/>
+  <dimension ref="A1:I37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5"/>
+  <cols>
+    <col min="2" max="2" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.54296875" style="117" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.7265625" style="115"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="7">
+        <v>1054</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="7">
+        <v>148</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="116">
+        <v>33344</v>
+      </c>
+      <c r="I1" s="115">
+        <v>11.25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="7">
+        <v>1056</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="7">
+        <v>121</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="116">
+        <v>29153</v>
+      </c>
+      <c r="I2" s="115">
+        <v>12.25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="7">
+        <v>1067</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" s="7">
+        <v>123</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" s="116">
+        <v>32040</v>
+      </c>
+      <c r="I3" s="115">
+        <v>14.55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="7">
+        <v>1075</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" s="7">
+        <v>126</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H4" s="116">
+        <v>33823</v>
+      </c>
+      <c r="I4" s="115">
+        <v>11.25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="7">
+        <v>1078</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" s="7">
+        <v>101</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H5" s="116">
+        <v>31503</v>
+      </c>
+      <c r="I5" s="115">
+        <v>10.199999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="7">
+        <v>1152</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" s="7">
+        <v>118</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H6" s="116">
+        <v>32894</v>
+      </c>
+      <c r="I6" s="115">
+        <v>12.25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="7">
+        <v>1196</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F7" s="7">
+        <v>289</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7" s="116">
+        <v>35886</v>
+      </c>
+      <c r="I7" s="115">
+        <v>9.9499999999999993</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="7">
+        <v>1284</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8" s="7">
+        <v>124</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H8" s="116">
+        <v>31051</v>
+      </c>
+      <c r="I8" s="115">
+        <v>12.3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="7">
+        <v>1290</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F9" s="7">
+        <v>113</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H9" s="116">
+        <v>31050</v>
+      </c>
+      <c r="I9" s="115">
+        <v>13.25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="7">
+        <v>1293</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="F10" s="7">
+        <v>205</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H10" s="116">
+        <v>30939</v>
+      </c>
+      <c r="I10" s="115">
+        <v>10.199999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="7">
+        <v>1299</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="F11" s="7">
+        <v>127</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H11" s="116">
+        <v>32863</v>
+      </c>
+      <c r="I11" s="115">
+        <v>12.2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="7">
+        <v>1302</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F12" s="7">
+        <v>139</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H12" s="116">
+        <v>30900</v>
+      </c>
+      <c r="I12" s="115">
+        <v>14.25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="7">
+        <v>1310</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="F13" s="7">
+        <v>137</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H13" s="116">
+        <v>31689</v>
+      </c>
+      <c r="I13" s="115">
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="7">
+        <v>1329</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F14" s="7">
+        <v>151</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H14" s="116">
+        <v>32561</v>
+      </c>
+      <c r="I14" s="115">
+        <v>10.35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="7">
+        <v>1333</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="F15" s="7">
+        <v>122</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H15" s="116">
+        <v>32979</v>
+      </c>
+      <c r="I15" s="115">
+        <v>10.15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="7">
+        <v>1368</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="F16" s="7">
+        <v>132</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H16" s="116">
+        <v>30386</v>
+      </c>
+      <c r="I16" s="115">
+        <v>12.25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="7">
+        <v>1509</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="F17" s="7">
+        <v>135</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H17" s="116">
+        <v>31217</v>
+      </c>
+      <c r="I17" s="115">
+        <v>13.25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="7">
+        <v>1516</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="F18" s="7">
+        <v>105</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H18" s="116">
+        <v>31112</v>
+      </c>
+      <c r="I18" s="115">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="7">
+        <v>1529</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="F19" s="7">
+        <v>129</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H19" s="116">
+        <v>31805</v>
+      </c>
+      <c r="I19" s="115">
+        <v>11.3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="7">
+        <v>1656</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="F20" s="7">
+        <v>149</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H20" s="116">
+        <v>32125</v>
+      </c>
+      <c r="I20" s="115">
+        <v>12.35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="7">
+        <v>1672</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F21" s="7">
+        <v>114</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H21" s="116">
+        <v>32979</v>
+      </c>
+      <c r="I21" s="115">
+        <v>11.9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="7">
+        <v>1673</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="F22" s="7">
+        <v>112</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H22" s="116">
+        <v>33688</v>
+      </c>
+      <c r="I22" s="115">
+        <v>11.85</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" s="7">
+        <v>1676</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="F23" s="7">
+        <v>115</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H23" s="116">
+        <v>29885</v>
+      </c>
+      <c r="I23" s="115">
+        <v>10.75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" s="7">
+        <v>1721</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="F24" s="7">
+        <v>102</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H24" s="116">
+        <v>33091</v>
+      </c>
+      <c r="I24" s="115">
+        <v>9.75</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" s="7">
+        <v>1723</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="F25" s="7">
+        <v>145</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H25" s="116">
+        <v>28531</v>
+      </c>
+      <c r="I25" s="115">
+        <v>13.95</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" s="7">
+        <v>1758</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F26" s="7">
+        <v>107</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H26" s="116">
+        <v>30028</v>
+      </c>
+      <c r="I26" s="115">
+        <v>11.2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" s="7">
+        <v>1792</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="F27" s="7">
+        <v>111</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H27" s="116">
+        <v>33231</v>
+      </c>
+      <c r="I27" s="115">
+        <v>10.3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" s="7">
+        <v>1814</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="F28" s="7">
+        <v>103</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H28" s="116">
+        <v>32571</v>
+      </c>
+      <c r="I28" s="115">
+        <v>12.25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" s="7">
+        <v>1908</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="F29" s="7">
+        <v>152</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H29" s="116">
+        <v>30817</v>
+      </c>
+      <c r="I29" s="115">
+        <v>10.25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" s="7">
+        <v>1931</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="F30" s="7">
+        <v>110</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H30" s="116">
+        <v>32679</v>
+      </c>
+      <c r="I30" s="115">
+        <v>9.85</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" s="7">
+        <v>1960</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="F31" s="7">
+        <v>150</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H31" s="116">
+        <v>31729</v>
+      </c>
+      <c r="I31" s="115">
+        <v>11.65</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" s="7">
+        <v>1964</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="F32" s="7">
+        <v>108</v>
+      </c>
+      <c r="G32" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H32" s="116">
+        <v>33559</v>
+      </c>
+      <c r="I32" s="115">
+        <v>9.25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" s="7">
+        <v>1975</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="F33" s="7">
+        <v>125</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H33" s="116">
+        <v>35125</v>
+      </c>
+      <c r="I33" s="115">
+        <v>9.25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" s="7">
+        <v>1983</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="F34" s="7">
+        <v>154</v>
+      </c>
+      <c r="G34" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H34" s="116">
+        <v>35609</v>
+      </c>
+      <c r="I34" s="115">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" s="7">
+        <v>1990</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="F35" s="7">
+        <v>198</v>
+      </c>
+      <c r="G35" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H35" s="116">
+        <v>35840</v>
+      </c>
+      <c r="I35" s="115">
+        <v>10.95</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36" s="7">
+        <v>1995</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="F36" s="7">
+        <v>198</v>
+      </c>
+      <c r="G36" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H36" s="116">
+        <v>35855</v>
+      </c>
+      <c r="I36" s="115">
+        <v>11.75</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37" s="7">
+        <v>1999</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="F37" s="7">
+        <v>428</v>
+      </c>
+      <c r="G37" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H37" s="116">
+        <v>35981</v>
+      </c>
+      <c r="I37" s="115">
+        <v>10.15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <sheetPr codeName="Sheet18"/>
   <dimension ref="A1:I37"/>
@@ -13919,6 +15014,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE727711-D0A2-4196-A6AA-50DDE55C0A6F}">
+  <sheetPr codeName="Sheet19"/>
   <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
@@ -15066,10 +16162,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="13" thickBot="1"/>
     <row r="2" spans="1:2" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A2" s="128" t="s">
+      <c r="A2" s="132" t="s">
         <v>231</v>
       </c>
-      <c r="B2" s="129"/>
+      <c r="B2" s="133"/>
     </row>
     <row r="3" spans="1:2" ht="16.5" thickTop="1" thickBot="1">
       <c r="A3" s="60" t="s">
@@ -15121,6 +16217,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7F7437D-A8FC-427C-8A49-940F6F4A8FBE}">
+  <sheetPr codeName="Sheet20"/>
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
@@ -15141,10 +16238,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="13" thickBot="1"/>
     <row r="2" spans="1:2" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A2" s="128" t="s">
+      <c r="A2" s="132" t="s">
         <v>231</v>
       </c>
-      <c r="B2" s="129"/>
+      <c r="B2" s="133"/>
     </row>
     <row r="3" spans="1:2" ht="16.5" thickTop="1" thickBot="1">
       <c r="A3" s="60" t="s">
@@ -15309,6 +16406,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87A99380-3415-42C6-8C41-613698A280FA}">
+  <sheetPr codeName="Sheet21"/>
   <dimension ref="B2:F19"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
@@ -15494,6 +16592,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E90CB938-F6AF-4391-A249-F7B9CAEC4582}">
+  <sheetPr codeName="Sheet22"/>
   <dimension ref="B1:G18"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">

</xml_diff>